<commit_message>
Adding testdata folder and report folder
</commit_message>
<xml_diff>
--- a/testdata/TestData_maintenance.xlsx
+++ b/testdata/TestData_maintenance.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="63">
   <si>
     <t>private</t>
   </si>
@@ -153,12 +153,6 @@
     <t>TestCaseId</t>
   </si>
   <si>
-    <t>TC_003</t>
-  </si>
-  <si>
-    <t>TC_004</t>
-  </si>
-  <si>
     <t>TestType</t>
   </si>
   <si>
@@ -196,6 +190,30 @@
   </si>
   <si>
     <t>Account email should be changed</t>
+  </si>
+  <si>
+    <t>ACMO-0001</t>
+  </si>
+  <si>
+    <t>ACMO-0002</t>
+  </si>
+  <si>
+    <t>ACMO-0003</t>
+  </si>
+  <si>
+    <t>ACMO-0004</t>
+  </si>
+  <si>
+    <t>Test case 1</t>
+  </si>
+  <si>
+    <t>Test case 2</t>
+  </si>
+  <si>
+    <t>Test case 3</t>
+  </si>
+  <si>
+    <t>Test case 4</t>
   </si>
 </sst>
 </file>
@@ -651,10 +669,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,13 +692,13 @@
         <v>41</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>17</v>
@@ -689,7 +707,7 @@
         <v>18</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>19</v>
@@ -700,16 +718,16 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>20</v>
@@ -724,24 +742,24 @@
         <v>24</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="51" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>22</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>21</v>
@@ -753,19 +771,21 @@
         <v>24</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B4" s="4"/>
+      <c r="A4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>59</v>
+      </c>
       <c r="C4" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>20</v>
@@ -781,11 +801,13 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B5" s="1"/>
+        <v>56</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="C5" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>22</v>
@@ -801,6 +823,40 @@
         <v>0</v>
       </c>
       <c r="I5" s="8"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>